<commit_message>
atualizacao 2a RQ 2024-2028
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2023/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2023/crescimento_mercado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arquivos Locais\codigos-R\epe4md\inst\dados_premissas\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arquivos Locais\projetos_r\epe4md-2rq2028\inst\dados_premissas\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3E5E75-6EB0-4A3E-A7B3-1CE01A1286A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADD6F5F-64BC-4292-A099-C40BA3611C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -376,15 +376,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -517,7 +517,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>2.0000000000000018E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
@@ -527,7 +527,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>2.200000000000002E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
@@ -537,7 +537,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>2.2999999999999909E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
@@ -547,7 +547,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>2.4999999999999911E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
@@ -557,7 +557,7 @@
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>2.9999999999999805E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
@@ -567,7 +567,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>3.0000000000000249E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
@@ -577,7 +577,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>3.0000000000000249E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
@@ -587,7 +587,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>3.0000000000000027E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
@@ -597,7 +597,7 @@
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>2.9999999999999805E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
@@ -607,7 +607,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>3.0000000000000249E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
@@ -617,7 +617,7 @@
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>3.0000000000000027E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
@@ -627,7 +627,7 @@
         <v>2035</v>
       </c>
       <c r="B27">
-        <v>2.9999999999999805E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
@@ -637,7 +637,7 @@
         <v>2036</v>
       </c>
       <c r="B28">
-        <v>3.0000000000000249E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
@@ -647,7 +647,7 @@
         <v>2037</v>
       </c>
       <c r="B29">
-        <v>3.0000000000000027E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
@@ -657,7 +657,7 @@
         <v>2038</v>
       </c>
       <c r="B30">
-        <v>2.9999999999999805E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
@@ -667,7 +667,7 @@
         <v>2039</v>
       </c>
       <c r="B31">
-        <v>3.0000000000000027E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
@@ -677,7 +677,7 @@
         <v>2040</v>
       </c>
       <c r="B32">
-        <v>3.0000000000000027E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
@@ -687,7 +687,7 @@
         <v>2041</v>
       </c>
       <c r="B33">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>2042</v>
       </c>
       <c r="B34">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -703,7 +703,7 @@
         <v>2043</v>
       </c>
       <c r="B35">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -711,7 +711,7 @@
         <v>2044</v>
       </c>
       <c r="B36">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -719,7 +719,7 @@
         <v>2045</v>
       </c>
       <c r="B37">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
         <v>2046</v>
       </c>
       <c r="B38">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>2047</v>
       </c>
       <c r="B39">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -743,7 +743,7 @@
         <v>2048</v>
       </c>
       <c r="B40">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>2049</v>
       </c>
       <c r="B41">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -759,7 +759,87 @@
         <v>2050</v>
       </c>
       <c r="B42">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2051</v>
+      </c>
+      <c r="B43">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2052</v>
+      </c>
+      <c r="B44">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2053</v>
+      </c>
+      <c r="B45">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2054</v>
+      </c>
+      <c r="B46">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2055</v>
+      </c>
+      <c r="B47">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2056</v>
+      </c>
+      <c r="B48">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2057</v>
+      </c>
+      <c r="B49">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2058</v>
+      </c>
+      <c r="B50">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2059</v>
+      </c>
+      <c r="B51">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2060</v>
+      </c>
+      <c r="B52">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Base para o PLAN 2029 e inclusão de dois novos parâmetros: receita bônus e alteração da participação das fontes.
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2023/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2023/crescimento_mercado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arquivos Locais\projetos_r\epe4md-2rq2028\inst\dados_premissas\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos_r\epe4md\inst\dados_premissas\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADD6F5F-64BC-4292-A099-C40BA3611C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964A6D28-9C53-4480-9A81-6DF6F9B8CC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -378,8 +378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -517,7 +517,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>2.1999999999999999E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>

</xml_diff>

<commit_message>
tx crescimento longo prazo
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2023/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2023/crescimento_mercado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos_r\epe4md\inst\dados_premissas\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964A6D28-9C53-4480-9A81-6DF6F9B8CC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CCBAA8-457B-4CCB-BF37-508E1F44F18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -376,18 +376,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,7 +395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -403,7 +403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -411,7 +411,7 @@
         <v>3.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -419,7 +419,7 @@
         <v>1.9199999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -427,7 +427,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -435,7 +435,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -443,7 +443,7 @@
         <v>-3.7699999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -451,7 +451,7 @@
         <v>-3.5900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -459,7 +459,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -467,7 +467,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -475,7 +475,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -483,323 +483,323 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
       <c r="B13" s="1">
         <v>4.6194216206421279E-2</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>0.03</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2024</v>
       </c>
-      <c r="B16">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>2.7451651971668989E-2</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2025</v>
       </c>
-      <c r="B17">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>2.9352266959988826E-2</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2026</v>
       </c>
-      <c r="B18">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>3.135258199435631E-2</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2027</v>
       </c>
-      <c r="B19">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>3.3298534411311698E-2</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2028</v>
       </c>
-      <c r="B20">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="1">
+        <v>3.5230250068047253E-2</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2029</v>
       </c>
-      <c r="B21">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="1">
+        <v>3.7244072645180371E-2</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2030</v>
       </c>
-      <c r="B22">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>3.9052382137174435E-2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2031</v>
       </c>
-      <c r="B23">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>4.0576022724664984E-2</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2032</v>
       </c>
-      <c r="B24">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>4.0664697033623742E-2</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2033</v>
       </c>
-      <c r="B25">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>4.0811931128108547E-2</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2034</v>
       </c>
-      <c r="B26">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>4.0676137059960427E-2</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2035</v>
       </c>
-      <c r="B27">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>4.040932346010484E-2</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2036</v>
       </c>
-      <c r="B28">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>4.0151149786510798E-2</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2037</v>
       </c>
-      <c r="B29">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>3.9927942873361433E-2</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2038</v>
       </c>
-      <c r="B30">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>3.978586583595467E-2</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2039</v>
       </c>
-      <c r="B31">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="1">
+        <v>3.9631024928610481E-2</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2040</v>
       </c>
-      <c r="B32">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4"/>
+      <c r="B32" s="1">
+        <v>3.9398816979326456E-2</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2041</v>
       </c>
-      <c r="B33">
-        <v>2.5999999999999999E-2</v>
+      <c r="B33" s="1">
+        <v>3.9121819430174121E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2042</v>
       </c>
-      <c r="B34">
-        <v>2.5999999999999999E-2</v>
+      <c r="B34" s="1">
+        <v>3.8820422967829948E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2043</v>
       </c>
-      <c r="B35">
-        <v>2.5999999999999999E-2</v>
+      <c r="B35" s="1">
+        <v>3.8529506722019491E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2044</v>
       </c>
-      <c r="B36">
-        <v>2.5999999999999999E-2</v>
+      <c r="B36" s="1">
+        <v>3.8289338002959639E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2045</v>
       </c>
-      <c r="B37">
-        <v>2.5999999999999999E-2</v>
+      <c r="B37" s="1">
+        <v>3.8134138778175064E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2046</v>
       </c>
-      <c r="B38">
-        <v>2.5999999999999999E-2</v>
+      <c r="B38" s="1">
+        <v>3.8073655849808263E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2047</v>
       </c>
-      <c r="B39">
-        <v>2.5999999999999999E-2</v>
+      <c r="B39" s="1">
+        <v>3.8071616838173394E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2048</v>
       </c>
-      <c r="B40">
-        <v>2.5999999999999999E-2</v>
+      <c r="B40" s="1">
+        <v>3.8091083280195059E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2049</v>
       </c>
-      <c r="B41">
-        <v>2.5999999999999999E-2</v>
+      <c r="B41" s="1">
+        <v>3.8146600936493913E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2050</v>
       </c>
-      <c r="B42">
-        <v>2.5999999999999999E-2</v>
+      <c r="B42" s="1">
+        <v>3.8265243583335273E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2051</v>
       </c>
-      <c r="B43">
-        <v>2.5999999999999999E-2</v>
+      <c r="B43" s="1">
+        <v>3.8442567895484059E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2052</v>
       </c>
-      <c r="B44">
-        <v>2.5999999999999999E-2</v>
+      <c r="B44" s="1">
+        <v>3.8669283676193045E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2053</v>
       </c>
-      <c r="B45">
-        <v>2.5999999999999999E-2</v>
+      <c r="B45" s="1">
+        <v>3.8924872761365803E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2054</v>
       </c>
-      <c r="B46">
-        <v>2.5999999999999999E-2</v>
+      <c r="B46" s="1">
+        <v>3.9163729435646166E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2055</v>
       </c>
-      <c r="B47">
-        <v>2.5999999999999999E-2</v>
+      <c r="B47" s="1">
+        <v>3.9344304288583487E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revert "tx crescimento longo prazo"
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2023/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2023/crescimento_mercado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos_r\epe4md\inst\dados_premissas\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CCBAA8-457B-4CCB-BF37-508E1F44F18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964A6D28-9C53-4480-9A81-6DF6F9B8CC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -376,18 +376,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,7 +395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -403,7 +403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -411,7 +411,7 @@
         <v>3.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -419,7 +419,7 @@
         <v>1.9199999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -427,7 +427,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -435,7 +435,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -443,7 +443,7 @@
         <v>-3.7699999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -451,7 +451,7 @@
         <v>-3.5900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -459,7 +459,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -467,7 +467,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -475,7 +475,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -483,323 +483,323 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
       <c r="B13" s="1">
         <v>4.6194216206421279E-2</v>
       </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>0.03</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2024</v>
       </c>
-      <c r="B16" s="1">
-        <v>2.7451651971668989E-2</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2025</v>
       </c>
-      <c r="B17" s="1">
-        <v>2.9352266959988826E-2</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2026</v>
       </c>
-      <c r="B18" s="1">
-        <v>3.135258199435631E-2</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2027</v>
       </c>
-      <c r="B19" s="1">
-        <v>3.3298534411311698E-2</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2028</v>
       </c>
-      <c r="B20" s="1">
-        <v>3.5230250068047253E-2</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2029</v>
       </c>
-      <c r="B21" s="1">
-        <v>3.7244072645180371E-2</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2030</v>
       </c>
-      <c r="B22" s="1">
-        <v>3.9052382137174435E-2</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2031</v>
       </c>
-      <c r="B23" s="1">
-        <v>4.0576022724664984E-2</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2032</v>
       </c>
-      <c r="B24" s="1">
-        <v>4.0664697033623742E-2</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2033</v>
       </c>
-      <c r="B25" s="1">
-        <v>4.0811931128108547E-2</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2034</v>
       </c>
-      <c r="B26" s="1">
-        <v>4.0676137059960427E-2</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2035</v>
       </c>
-      <c r="B27" s="1">
-        <v>4.040932346010484E-2</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2036</v>
       </c>
-      <c r="B28" s="1">
-        <v>4.0151149786510798E-2</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2037</v>
       </c>
-      <c r="B29" s="1">
-        <v>3.9927942873361433E-2</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2038</v>
       </c>
-      <c r="B30" s="1">
-        <v>3.978586583595467E-2</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2039</v>
       </c>
-      <c r="B31" s="1">
-        <v>3.9631024928610481E-2</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2040</v>
       </c>
-      <c r="B32" s="1">
-        <v>3.9398816979326456E-2</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
+      <c r="B32">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2041</v>
       </c>
-      <c r="B33" s="1">
-        <v>3.9121819430174121E-2</v>
+      <c r="B33">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2042</v>
       </c>
-      <c r="B34" s="1">
-        <v>3.8820422967829948E-2</v>
+      <c r="B34">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2043</v>
       </c>
-      <c r="B35" s="1">
-        <v>3.8529506722019491E-2</v>
+      <c r="B35">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2044</v>
       </c>
-      <c r="B36" s="1">
-        <v>3.8289338002959639E-2</v>
+      <c r="B36">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2045</v>
       </c>
-      <c r="B37" s="1">
-        <v>3.8134138778175064E-2</v>
+      <c r="B37">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2046</v>
       </c>
-      <c r="B38" s="1">
-        <v>3.8073655849808263E-2</v>
+      <c r="B38">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2047</v>
       </c>
-      <c r="B39" s="1">
-        <v>3.8071616838173394E-2</v>
+      <c r="B39">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2048</v>
       </c>
-      <c r="B40" s="1">
-        <v>3.8091083280195059E-2</v>
+      <c r="B40">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2049</v>
       </c>
-      <c r="B41" s="1">
-        <v>3.8146600936493913E-2</v>
+      <c r="B41">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2050</v>
       </c>
-      <c r="B42" s="1">
-        <v>3.8265243583335273E-2</v>
+      <c r="B42">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2051</v>
       </c>
-      <c r="B43" s="1">
-        <v>3.8442567895484059E-2</v>
+      <c r="B43">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2052</v>
       </c>
-      <c r="B44" s="1">
-        <v>3.8669283676193045E-2</v>
+      <c r="B44">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2053</v>
       </c>
-      <c r="B45" s="1">
-        <v>3.8924872761365803E-2</v>
+      <c r="B45">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2054</v>
       </c>
-      <c r="B46" s="1">
-        <v>3.9163729435646166E-2</v>
+      <c r="B46">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2055</v>
       </c>
-      <c r="B47" s="1">
-        <v>3.9344304288583487E-2</v>
+      <c r="B47">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
reversão pib 2a RQ 2024-28
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2023/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2023/crescimento_mercado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos_r\epe4md\inst\dados_premissas\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964A6D28-9C53-4480-9A81-6DF6F9B8CC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EB30A3-BC4C-4458-AA70-64409CF274CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -378,8 +378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -517,7 +517,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>3.2000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>

</xml_diff>